<commit_message>
Se tunearon los controladores
</commit_message>
<xml_diff>
--- a/recta_para_feedfoward.xlsx
+++ b/recta_para_feedfoward.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juan\Documents\GitHub\Proyecto_de_Graduacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9A1AAD-9268-4DB6-AB18-2ADF8B4420E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4EFCDD-2889-471B-8874-2CFA2BF94EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{39748E5E-E720-46D1-8553-D430143A0602}"/>
   </bookViews>
@@ -34,12 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>PWM</t>
   </si>
   <si>
     <t>RPM</t>
+  </si>
+  <si>
+    <t>rad/s</t>
   </si>
 </sst>
 </file>
@@ -145,15 +148,15 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RPM</c:v>
+                  <c:v>rad/s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -161,7 +164,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -172,11 +175,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -186,7 +189,21 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
               </a:ln>
@@ -198,8 +215,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.57836959100286001"/>
-                  <c:y val="0.1050553221483357"/>
+                  <c:x val="-4.3300899751956168E-2"/>
+                  <c:y val="-4.1243333982545469E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -232,139 +249,129 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$44</c:f>
+              <c:f>Sheet1!$A$10:$A$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="43"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>300</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>400</c:v>
+                  <c:v>1100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>500</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>600</c:v>
+                  <c:v>1300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>699</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>700</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>800</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>900</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1000</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1100</c:v>
+                  <c:v>1900</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1200</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1300</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1400</c:v>
+                  <c:v>2200</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1500</c:v>
+                  <c:v>2300</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1600</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1700</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1800</c:v>
+                  <c:v>2600</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1900</c:v>
+                  <c:v>2700</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2000</c:v>
+                  <c:v>2800</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2100</c:v>
+                  <c:v>2900</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2200</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2300</c:v>
+                  <c:v>3100</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2400</c:v>
+                  <c:v>3200</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2500</c:v>
+                  <c:v>3300</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2600</c:v>
+                  <c:v>3400</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2700</c:v>
+                  <c:v>3500</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2800</c:v>
+                  <c:v>3600</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2900</c:v>
+                  <c:v>3700</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3000</c:v>
+                  <c:v>3800</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3100</c:v>
+                  <c:v>3900</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3200</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3300</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>3400</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>3600</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>3700</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>3800</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>3900</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="42">
                   <c:v>4095</c:v>
                 </c:pt>
               </c:numCache>
@@ -372,138 +379,114 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$44</c:f>
+              <c:f>Sheet1!$C$10:$C$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="43"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>11.833332328521553</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>12.461650859239512</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>13.718287920675431</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>15.027284859671177</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>16.126842288427603</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>17.592918860102841</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>18.849555921538759</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>20.158552860534506</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>113</c:v>
+                  <c:v>21.467549799530254</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>119</c:v>
+                  <c:v>22.200588085367873</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>131</c:v>
+                  <c:v>23.980823922402084</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>143.5</c:v>
+                  <c:v>25.289820861397835</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>154</c:v>
+                  <c:v>27.227136331111538</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>168</c:v>
+                  <c:v>27.8554548618295</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>180</c:v>
+                  <c:v>29.740410453983376</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>192.5</c:v>
+                  <c:v>30.421088862261165</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>205</c:v>
+                  <c:v>32.358404331974867</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>212</c:v>
+                  <c:v>33.615041393410785</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>229</c:v>
+                  <c:v>34.924038332406532</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>241.5</c:v>
+                  <c:v>36.233035271402279</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>260</c:v>
+                  <c:v>38.117990863556159</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>266</c:v>
+                  <c:v>39.374627924992076</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>284</c:v>
+                  <c:v>40.735984741547654</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>290.5</c:v>
+                  <c:v>41.992621802983564</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>309</c:v>
+                  <c:v>43.249258864419488</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>321</c:v>
+                  <c:v>44.505895925855398</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>333.5</c:v>
+                  <c:v>45.867252742410983</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>346</c:v>
+                  <c:v>47.123889803846893</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>364</c:v>
+                  <c:v>48.380526865282818</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>376</c:v>
+                  <c:v>49.008845396000773</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>389</c:v>
+                  <c:v>50.31784233499652</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>401</c:v>
+                  <c:v>50.684361477915331</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>413</c:v>
+                  <c:v>50.684361477915331</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>425</c:v>
+                  <c:v>51.626839273992267</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>438</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>450</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>462</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>468</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>480.5</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>484</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>484</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>493</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>493</c:v>
+                  <c:v>51.626839273992267</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -511,7 +494,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D17D-4DE6-A992-B2EF58E038F9}"/>
+              <c16:uniqueId val="{00000002-C2BB-49A0-99EE-0DE5215E9DAE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -525,6 +508,367 @@
         </c:dLbls>
         <c:axId val="671685256"/>
         <c:axId val="671690176"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>RPM</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:trendline>
+                  <c:spPr>
+                    <a:ln w="19050" cap="rnd">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:prstDash val="sysDot"/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:trendlineType val="linear"/>
+                  <c:dispRSqr val="0"/>
+                  <c:dispEq val="0"/>
+                </c:trendline>
+                <c:trendline>
+                  <c:spPr>
+                    <a:ln w="19050" cap="rnd">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:prstDash val="sysDot"/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:trendlineType val="linear"/>
+                  <c:dispRSqr val="0"/>
+                  <c:dispEq val="1"/>
+                  <c:trendlineLbl>
+                    <c:layout>
+                      <c:manualLayout>
+                        <c:x val="-0.11645149469228577"/>
+                        <c:y val="3.6140341114604492E-2"/>
+                      </c:manualLayout>
+                    </c:layout>
+                    <c:numFmt formatCode="General" sourceLinked="0"/>
+                    <c:spPr>
+                      <a:noFill/>
+                      <a:ln>
+                        <a:noFill/>
+                      </a:ln>
+                      <a:effectLst/>
+                    </c:spPr>
+                    <c:txPr>
+                      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                      <a:lstStyle/>
+                      <a:p>
+                        <a:pPr>
+                          <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="65000"/>
+                                <a:lumOff val="35000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:defRPr>
+                        </a:pPr>
+                        <a:endParaRPr lang="es-GT"/>
+                      </a:p>
+                    </c:txPr>
+                  </c:trendlineLbl>
+                </c:trendline>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$10:$A$44</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="35"/>
+                      <c:pt idx="0">
+                        <c:v>700</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>800</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>900</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1000</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1100</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1200</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1300</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1400</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>1500</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>1600</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>1700</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>1800</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>1900</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>2000</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>2100</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>2200</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>2300</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>2400</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>2500</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>2600</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>2700</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>2800</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>2900</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>3000</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>3100</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>3200</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>3300</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>3400</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>3500</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>3600</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>3700</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>3800</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>3900</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>4000</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>4095</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$10:$B$44</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="35"/>
+                      <c:pt idx="0">
+                        <c:v>113</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>119</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>131</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>143.5</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>154</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>168</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>180</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>192.5</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>205</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>212</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>229</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>241.5</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>260</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>266</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>284</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>290.5</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>309</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>321</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>333.5</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>346</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>364</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>376</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>389</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>401</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>413</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>425</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>438</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>450</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>462</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>468</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>480.5</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>484</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>484</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>493</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>493</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-D17D-4DE6-A992-B2EF58E038F9}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="671685256"/>
@@ -702,7 +1046,477 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-GT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rad/s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-GT"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-894F-4200-B9EE-88908A2A8B31}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="712139952"/>
+        <c:axId val="712141264"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="712139952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="712141264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="712141264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="712139952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-GT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1258,20 +2072,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>428624</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>185737</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>169489</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>190499</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>557212</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>36139</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1291,6 +2621,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>233361</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>80961</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5774D0C-022D-484A-A6E1-51B3FC915CAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1596,364 +2962,745 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7AB0709-1EE2-46CA-AE99-9DEB808CC3EE}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AD11" sqref="AD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>A2+30</f>
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>100</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E44" si="0">A3+30</f>
+        <v>130</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>200</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>300</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>330</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>400</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>430</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>500</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>530</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>600</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>630</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>699</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>729</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>700</v>
       </c>
       <c r="B10">
         <v>113</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <f>B10*2*PI()/60</f>
+        <v>11.833332328521553</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>730</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>800</v>
       </c>
       <c r="B11">
         <v>119</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <f t="shared" ref="C11:C44" si="1">B11*2*PI()/60</f>
+        <v>12.461650859239512</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>830</v>
+      </c>
+      <c r="F11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>900</v>
       </c>
       <c r="B12">
         <v>131</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>13.718287920675431</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>930</v>
+      </c>
+      <c r="F12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1000</v>
       </c>
       <c r="B13">
         <v>143.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>15.027284859671177</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>1030</v>
+      </c>
+      <c r="F13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1100</v>
       </c>
       <c r="B14">
         <v>154</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>16.126842288427603</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1200</v>
       </c>
       <c r="B15">
         <v>168</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>17.592918860102841</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1300</v>
       </c>
       <c r="B16">
         <v>180</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>18.849555921538759</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1400</v>
       </c>
       <c r="B17">
         <v>192.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>20.158552860534506</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1500</v>
       </c>
       <c r="B18">
         <v>205</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>21.467549799530254</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1600</v>
       </c>
       <c r="B19">
         <v>212</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>22.200588085367873</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1700</v>
       </c>
       <c r="B20">
         <v>229</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>23.980823922402084</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1800</v>
       </c>
       <c r="B21">
         <v>241.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>25.289820861397835</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1900</v>
       </c>
       <c r="B22">
         <v>260</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>27.227136331111538</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2000</v>
       </c>
       <c r="B23">
         <v>266</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>27.8554548618295</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2100</v>
       </c>
       <c r="B24">
         <v>284</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>29.740410453983376</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>2130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2200</v>
       </c>
       <c r="B25">
         <v>290.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>30.421088862261165</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>2230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2300</v>
       </c>
       <c r="B26">
         <v>309</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>32.358404331974867</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>2330</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2400</v>
       </c>
       <c r="B27">
         <v>321</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>33.615041393410785</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>2430</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2500</v>
       </c>
       <c r="B28">
         <v>333.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>34.924038332406532</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>2530</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2600</v>
       </c>
       <c r="B29">
         <v>346</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>36.233035271402279</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>2630</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2700</v>
       </c>
       <c r="B30">
         <v>364</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>38.117990863556159</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>2730</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2800</v>
       </c>
       <c r="B31">
         <v>376</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>39.374627924992076</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>2830</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2900</v>
       </c>
       <c r="B32">
         <v>389</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>40.735984741547654</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>2930</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3000</v>
       </c>
       <c r="B33">
         <v>401</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>41.992621802983564</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3100</v>
       </c>
       <c r="B34">
         <v>413</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>43.249258864419488</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3200</v>
       </c>
       <c r="B35">
         <v>425</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>44.505895925855398</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3300</v>
       </c>
       <c r="B36">
         <v>438</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>45.867252742410983</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>3330</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>3400</v>
       </c>
       <c r="B37">
         <v>450</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>47.123889803846893</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>3430</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3500</v>
       </c>
       <c r="B38">
         <v>462</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>48.380526865282818</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>3530</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3600</v>
       </c>
       <c r="B39">
         <v>468</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>49.008845396000773</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>3630</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3700</v>
       </c>
       <c r="B40">
         <v>480.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <f t="shared" si="1"/>
+        <v>50.31784233499652</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>3730</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>3800</v>
       </c>
       <c r="B41">
         <v>484</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <f t="shared" si="1"/>
+        <v>50.684361477915331</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>3830</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3900</v>
       </c>
       <c r="B42">
         <v>484</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <f t="shared" si="1"/>
+        <v>50.684361477915331</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>3930</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>4000</v>
       </c>
       <c r="B43">
         <v>493</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <f t="shared" si="1"/>
+        <v>51.626839273992267</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>4030</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>4095</v>
       </c>
       <c r="B44">
         <v>493</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="1"/>
+        <v>51.626839273992267</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>4125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>